<commit_message>
updated Master and samples with new tabs for exercise 4.
</commit_message>
<xml_diff>
--- a/Fundementals/Data/BikeStoreSamples/BikeStoreSample01.xlsx
+++ b/Fundementals/Data/BikeStoreSamples/BikeStoreSample01.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Elevation\Excel\Fundementals\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEF8DCA-CD3E-454C-BBD1-C92EEA3948E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E56E70-5220-4AF0-AE19-9E4D7E56882E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="2280" yWindow="1605" windowWidth="24915" windowHeight="11385" firstSheet="0" activeTab="0" xr2:uid="{E731B28F-D92B-4ABF-AE71-A2BC403318D1}"/>
+    <x:workbookView xWindow="1425" yWindow="3060" windowWidth="26235" windowHeight="11385" firstSheet="0" activeTab="0" xr2:uid="{E731B28F-D92B-4ABF-AE71-A2BC403318D1}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="OrderDetailsData" sheetId="1" r:id="rId1"/>
+    <x:sheet name="YearlyIncome" sheetId="2" r:id="rId2"/>
+    <x:sheet name="MonthlyIncome" sheetId="3" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191029"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <x:si>
     <x:t>order_id</x:t>
   </x:si>
@@ -502,6 +504,18 @@
   </x:si>
   <x:si>
     <x:t>Electra Cruiser 1 - 2016/2017/2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Year</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Total </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Month</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -509,9 +523,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
+    <x:numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </x:numFmts>
-  <x:fonts count="3" x14ac:knownFonts="1">
+  <x:fonts count="4" x14ac:knownFonts="1">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
@@ -521,6 +535,13 @@
     </x:font>
     <x:font>
       <x:b/>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Calibri"/>
@@ -543,7 +564,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="1">
+  <x:borders count="2">
     <x:border>
       <x:left/>
       <x:right/>
@@ -551,22 +572,52 @@
       <x:bottom/>
       <x:diagonal/>
     </x:border>
+    <x:border>
+      <x:left style="thin">
+        <x:color indexed="64"/>
+      </x:left>
+      <x:right style="thin">
+        <x:color indexed="64"/>
+      </x:right>
+      <x:top style="thin">
+        <x:color indexed="64"/>
+      </x:top>
+      <x:bottom style="thin">
+        <x:color indexed="64"/>
+      </x:bottom>
+      <x:diagonal/>
+    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="44" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <x:xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <x:xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </x:cellXfs>
-  <x:cellStyles count="1">
+  <x:cellStyles count="2">
+    <x:cellStyle name="Currency" xfId="1" builtinId="4"/>
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -883,9 +934,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:P4723"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <x:selection activeCell="E9" sqref="E9"/>
-    </x:sheetView>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
@@ -4724,4 +4773,196 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{19B0669B-A8EB-4D1F-8021-CE894C392FA0}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D2"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="10" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.570312" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="17.425781" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="17" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="3" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="B1" s="3" t="n">
+        <x:v>2016</x:v>
+      </x:c>
+      <x:c r="C1" s="3" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="D1" s="3" t="n">
+        <x:v>2018</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="5" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B2" s="4" t="s"/>
+      <x:c r="C2" s="4" t="s"/>
+      <x:c r="D2" s="4" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{3DE0EF86-128A-403E-A565-B029CC7D118E}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:D14"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="10" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.570312" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="17.425781" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="17" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="3" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="B1" s="3" t="n">
+        <x:v>2016</x:v>
+      </x:c>
+      <x:c r="C1" s="3" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="D1" s="3" t="n">
+        <x:v>2018</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="5" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B2" s="4" t="s"/>
+      <x:c r="C2" s="4" t="s"/>
+      <x:c r="D2" s="4" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="5" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="4" t="s"/>
+      <x:c r="C3" s="4" t="s"/>
+      <x:c r="D3" s="4" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" s="4" t="s"/>
+      <x:c r="C4" s="4" t="s"/>
+      <x:c r="D4" s="4" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="5" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B5" s="4" t="s"/>
+      <x:c r="C5" s="4" t="s"/>
+      <x:c r="D5" s="4" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="5" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B6" s="4" t="s"/>
+      <x:c r="C6" s="4" t="s"/>
+      <x:c r="D6" s="4" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="5" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B7" s="4" t="s"/>
+      <x:c r="C7" s="4" t="s"/>
+      <x:c r="D7" s="4" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="5" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B8" s="4" t="s"/>
+      <x:c r="C8" s="4" t="s"/>
+      <x:c r="D8" s="4" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="5" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B9" s="4" t="s"/>
+      <x:c r="C9" s="4" t="s"/>
+      <x:c r="D9" s="4" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="5" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B10" s="4" t="s"/>
+      <x:c r="C10" s="4" t="s"/>
+      <x:c r="D10" s="4" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="5" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B11" s="4" t="s"/>
+      <x:c r="C11" s="4" t="s"/>
+      <x:c r="D11" s="4" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="5" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B12" s="4" t="s"/>
+      <x:c r="C12" s="4" t="s"/>
+      <x:c r="D12" s="4" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="5" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B13" s="4" t="s"/>
+      <x:c r="C13" s="4" t="s"/>
+      <x:c r="D13" s="4" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="3" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="B14" s="4" t="s"/>
+      <x:c r="C14" s="4" t="s"/>
+      <x:c r="D14" s="4" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>